<commit_message>
added bbb i2c dts!
</commit_message>
<xml_diff>
--- a/doc/i2c-test-doc.xlsx
+++ b/doc/i2c-test-doc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="general study" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="110">
   <si>
     <t xml:space="preserve">32k eeprom implemented</t>
   </si>
@@ -322,6 +322,111 @@
   <si>
     <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] </t>
   </si>
+  <si>
+    <t xml:space="preserve">if you use default kernel….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2c-1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">[dmotooka@ *BBB* :~] </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sudo sh -c "echo BB-I2C1 &gt; /sys/devices/bone_capemgr.9/slots"</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] ll i2c-*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 11:39 i2c-0 -&gt; ../../../devices/ocp.3/44e0b000.i2c/i2c-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 11:39 i2c-1 -&gt; ../../../devices/ocp.3/4819c000.i2c/i2c-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 11:45 i2c-2 -&gt; ../../../devices/ocp.3/4802a000.i2c/i2c-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] i2cdetect -r 0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] i2cdetect -r 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will probe file /dev/i2c-1 using read byte commands.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] i2cdetect -r 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50: -- -- -- -- -- -- -- -- -- -- -- -- -- -- -- -- </t>
+  </si>
+  <si>
+    <t xml:space="preserve">now my dts integration….</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :/sys/bus/i2c/devices] uname -a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linux beaglebone 4.4.68-moto #2 SMP Sat Jun 24 19:50:53 JST 2017 armv7l GNU/Linux</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :~] sudo sh -c "echo duper-i2c &gt; /sys/devices/platform/bone_capemgr/slots "</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 14:30 i2c-0 -&gt; ../../../devices/platform/ocp/44e0b000.i2c/i2c-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 14:30 i2c-1 -&gt; ../../../devices/platform/ocp/4802a000.i2c/i2c-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 14:30 i2c-2 -&gt; ../../../devices/platform/ocp/4819c000.i2c/i2c-2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">40: -- -- -- --</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> -- </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">-- -- -- -- -- -- ^C</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -330,7 +435,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="TakaoPGothic"/>
@@ -377,13 +482,26 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF3333"/>
+      <name val="TakaoGothic"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -420,7 +538,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,6 +551,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -442,6 +568,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF3333"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -456,9 +642,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>236160</xdr:colOff>
+      <xdr:colOff>235800</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>4320</xdr:rowOff>
+      <xdr:rowOff>3960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -467,13 +653,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="46431" t="28329" r="3630" b="0"/>
+        <a:srcRect l="46425" t="28325" r="3630" b="0"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16261200" y="1305000"/>
-          <a:ext cx="7977960" cy="7399800"/>
+          <a:ext cx="7977600" cy="7399440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -494,9 +680,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>174600</xdr:colOff>
+      <xdr:colOff>174240</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>123480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -506,7 +692,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24778080" y="4232880"/>
-          <a:ext cx="1456920" cy="2640960"/>
+          <a:ext cx="1456560" cy="2640600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -674,9 +860,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>257760</xdr:colOff>
+      <xdr:colOff>257400</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -685,13 +871,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="25728" t="14124" r="37299" b="7013"/>
+        <a:srcRect l="25724" t="14121" r="37295" b="7013"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7990200" y="1485000"/>
-          <a:ext cx="5983560" cy="8143920"/>
+          <a:ext cx="5983200" cy="8143560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -712,9 +898,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>340200</xdr:colOff>
+      <xdr:colOff>339840</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -724,7 +910,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13970520" y="6805080"/>
-          <a:ext cx="1457280" cy="1808280"/>
+          <a:ext cx="1456920" cy="1807920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -792,9 +978,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>117000</xdr:colOff>
+      <xdr:colOff>116640</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:rowOff>16920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -804,7 +990,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4717800" y="11623680"/>
-          <a:ext cx="1571400" cy="1808280"/>
+          <a:ext cx="1571040" cy="1807920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -904,9 +1090,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>470520</xdr:colOff>
+      <xdr:colOff>470160</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>149400</xdr:rowOff>
+      <xdr:rowOff>149040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -916,7 +1102,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5871600" y="14356800"/>
-          <a:ext cx="1456920" cy="1808280"/>
+          <a:ext cx="1456560" cy="1807920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1016,9 +1202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>17640</xdr:colOff>
+      <xdr:colOff>17280</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1028,7 +1214,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6675840" y="23697000"/>
-          <a:ext cx="1571400" cy="1808280"/>
+          <a:ext cx="1571040" cy="1807920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1160,9 +1346,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>74520</xdr:colOff>
+      <xdr:colOff>74160</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>115560</xdr:rowOff>
+      <xdr:rowOff>115200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1171,13 +1357,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId8"/>
-        <a:srcRect l="33909" t="56784" r="29758" b="22625"/>
+        <a:srcRect l="33906" t="56777" r="29754" b="22621"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="676080"/>
-          <a:ext cx="6932520" cy="2125440"/>
+          <a:ext cx="6932160" cy="2125080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1198,9 +1384,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>219600</xdr:colOff>
+      <xdr:colOff>219240</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1209,13 +1395,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId9"/>
-        <a:srcRect l="35520" t="30306" r="30980" b="46432"/>
+        <a:srcRect l="35516" t="30303" r="30976" b="46425"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3501720"/>
-          <a:ext cx="6391800" cy="2402280"/>
+          <a:ext cx="6391440" cy="2401920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1236,9 +1422,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>465480</xdr:colOff>
+      <xdr:colOff>465120</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>69480</xdr:rowOff>
+      <xdr:rowOff>69120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1247,13 +1433,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId10"/>
-        <a:srcRect l="34242" t="55430" r="30970" b="26355"/>
+        <a:srcRect l="34238" t="55423" r="30967" b="26352"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6563880"/>
-          <a:ext cx="6637680" cy="1881000"/>
+          <a:ext cx="6637320" cy="1880640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1274,9 +1460,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>268200</xdr:colOff>
+      <xdr:colOff>267840</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>29880</xdr:rowOff>
+      <xdr:rowOff>29520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1286,7 +1472,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="686160" y="26583120"/>
-          <a:ext cx="6440040" cy="1491840"/>
+          <a:ext cx="6439680" cy="1491480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1391,9 +1577,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>592920</xdr:colOff>
+      <xdr:colOff>592560</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1402,13 +1588,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="30454" t="13893" r="21612" b="4239"/>
+        <a:srcRect l="30452" t="13893" r="21610" b="4239"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="335160" y="122040"/>
-          <a:ext cx="6760080" cy="7342200"/>
+          <a:ext cx="6658200" cy="7341840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1429,9 +1615,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>624600</xdr:colOff>
+      <xdr:colOff>624240</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1440,8 +1626,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7265880" y="4111920"/>
-          <a:ext cx="2299320" cy="946440"/>
+          <a:off x="7164360" y="4111920"/>
+          <a:ext cx="2260800" cy="946080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1573,9 +1759,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>674280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>134280</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1584,8 +1770,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="813240" y="10404360"/>
-          <a:ext cx="2299320" cy="946440"/>
+          <a:off x="800640" y="10404360"/>
+          <a:ext cx="2273400" cy="946080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1626,329 +1812,7 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>I</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>c</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>0</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>s</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>t</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>x</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>p</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>s</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>d</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
+            <a:t>I2c-0 is not exposed on </a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -1980,287 +1844,7 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>t</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>h</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>x</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>p</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>s</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>h</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>d</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>r</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>!</a:t>
+            <a:t>the expansion header!</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -2292,371 +1876,7 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>O</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>l</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>y</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>c</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>1</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>,</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>s</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>v</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>l</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>b</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>l</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>.</a:t>
+            <a:t>Only i2c-1, 2 is available.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -2683,9 +1903,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>475560</xdr:colOff>
+      <xdr:colOff>475200</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>143640</xdr:rowOff>
+      <xdr:rowOff>143280</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2694,8 +1914,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8742600" y="10088640"/>
-          <a:ext cx="2299320" cy="946440"/>
+          <a:off x="8615880" y="10088640"/>
+          <a:ext cx="2260440" cy="946080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2736,329 +1956,7 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>E</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>p</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>r</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>m</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>d</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>t</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>h</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>r</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>m</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>d</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>u</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>l</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>s</a:t>
+            <a:t>Eeprom and other modules</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -3090,175 +1988,7 @@
               </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>a</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>r</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>e</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>o</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>n</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>i</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>2</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>c</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>0</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Times New Roman"/>
-            </a:rPr>
-            <a:t>.</a:t>
+            <a:t>are on i2c-0.</a:t>
           </a:r>
           <a:endParaRPr b="0" lang="en-US" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
@@ -3290,9 +2020,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>535320</xdr:colOff>
+      <xdr:colOff>534960</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3301,13 +2031,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="22795" t="28052" r="10787" b="65546"/>
+        <a:srcRect l="22792" t="28049" r="10784" b="65535"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="488160"/>
-          <a:ext cx="8663040" cy="621000"/>
+          <a:ext cx="8535960" cy="620640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3328,9 +2058,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>446040</xdr:colOff>
+      <xdr:colOff>445680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>84960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3339,13 +2069,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="23022" t="71453" r="11241" b="23131"/>
+        <a:srcRect l="23019" t="71442" r="11241" b="23127"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1673280"/>
-          <a:ext cx="8573760" cy="525240"/>
+          <a:ext cx="8446680" cy="524880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3366,9 +2096,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>158400</xdr:colOff>
+      <xdr:colOff>158040</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>104400</xdr:rowOff>
+      <xdr:rowOff>104040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3377,13 +2107,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="23097" t="44483" r="7444" b="49609"/>
+        <a:srcRect l="23094" t="44476" r="7444" b="49602"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="2782440"/>
-          <a:ext cx="9059400" cy="573120"/>
+          <a:ext cx="8919360" cy="572760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3409,9 +2139,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>594000</xdr:colOff>
+      <xdr:colOff>593640</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>37800</xdr:rowOff>
+      <xdr:rowOff>37440</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3420,13 +2150,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="31221" t="27553" r="20502" b="9629"/>
+        <a:srcRect l="31218" t="27549" r="20499" b="9629"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="445680" y="152640"/>
-          <a:ext cx="6650640" cy="4924440"/>
+          <a:ext cx="6548760" cy="4924080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3448,8 +2178,8 @@
   </sheetPr>
   <dimension ref="A2:M161"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A145" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N80" activeCellId="0" sqref="N80"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A156" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M175" activeCellId="0" sqref="M175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3834,9 +2564,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1711711711712"/>
-  </cols>
   <sheetData>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -3909,14 +2636,11 @@
   </sheetPr>
   <dimension ref="A25:A27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O49" activeCellId="0" sqref="O49"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1711711711712"/>
-  </cols>
   <sheetData>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -3950,24 +2674,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:D40"/>
+  <dimension ref="A3:D173"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A158" activeCellId="0" sqref="A158"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1711711711712"/>
-  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="2" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3981,7 +2702,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4146,6 +2867,653 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="114" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D121" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D122" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B126" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C126" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="2" t="s">
         <v>89</v>
       </c>
     </row>
@@ -4172,9 +3540,6 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1711711711712"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
i2c-1 eeprom test okgit add i2c-test-doc.xlsx
</commit_message>
<xml_diff>
--- a/doc/i2c-test-doc.xlsx
+++ b/doc/i2c-test-doc.xlsx
@@ -5,14 +5,15 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="general study" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="pins" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="omap ref" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="impl" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="ascii code table" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="eeprom test" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="ascii code table" sheetId="6" state="visible" r:id="rId7"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="157">
   <si>
     <t xml:space="preserve">32k eeprom implemented</t>
   </si>
@@ -386,7 +387,7 @@
     <t xml:space="preserve">Linux beaglebone 4.4.68-moto #2 SMP Sat Jun 24 19:50:53 JST 2017 armv7l GNU/Linux</t>
   </si>
   <si>
-    <t xml:space="preserve">[dmotooka@ *BBB* :~] sudo sh -c "echo duper-i2c &gt; /sys/devices/platform/bone_capemgr/slots "</t>
+    <t xml:space="preserve">sudo sh -c "echo duper-i2c &gt; /sys/devices/platform/bone_capemgr/slots "</t>
   </si>
   <si>
     <t xml:space="preserve">lrwxrwxrwx 1 root root 0 Jul  1 14:30 i2c-0 -&gt; ../../../devices/platform/ocp/44e0b000.i2c/i2c-0</t>
@@ -445,6 +446,183 @@
   <si>
     <t xml:space="preserve"> 4: P-O-L-   0 Override Board Name,00A0,Override Manuf,duper-i2c</t>
   </si>
+  <si>
+    <t xml:space="preserve">i2c device on i2c2:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :~] ls /sys/bus/i2c/devices/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-0024  0-0034  0-0050  0-0070  2-0054  2-0055  2-0056  2-0057  i2c-0  i2c-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo sh -c "echo 24c256 0x50 &gt; /sys/bus/i2c/devices/i2c-2/new_device"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmesg | tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 2915.907375] at24 2-0050: 32768 byte 24c256 EEPROM, writable, 1 bytes/write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 2915.926529] i2c i2c-2: new_device: Instantiated device 24c256 at 0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-0024  0-0050  2-0050  2-0055  2-0057  i2c-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-0034  0-0070  2-0054  2-0056  i2c-0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo sh -c "echo \"This is a text to be stored in out EEPROM\" &gt; /sys/bus/i2c/devices/2-0050/eeprom"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo cat /sys/bus/i2c/devices/2-0050/eeprom | hexdump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000000  54 68 69 73 20 69 73 20  61 20 74 65 78 74 20 74  |This is a text t|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000010  6f 20 62 65 20 73 74 6f  72 65 64 20 69 6e 20 6f  |o be stored in o|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000020  75 74 20 45 45 50 52 4f  4d 0a ff ff ff ff ff ff  |ut EEPROM.......|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000030  ff ff ff ff ff ff ff ff  ff ff ff ff ff ff ff ff  |................|</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo sh -c "echo 0x50 &gt; /sys/bus/i2c/devices/i2c-2/delete_device"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :~] dmesg |tail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 3626.840042] i2c i2c-2: delete_device: Deleting device 24c256 at 0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2c device on i2c1:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">i2cdetect -r 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">50: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">50</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> -- -- -- -- -- -- -- -- -- -- -- -- -- -- -- </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">sudo sh -c "echo 24c256 0x50 &gt; /sys/bus/i2c/devices/i2c-1/new_device"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmesg |tail -n15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 3745.330571] i2c i2c-2: new_device: Instantiated device 24c256 at 0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 3777.415855] i2c i2c-2: delete_device: Deleting device 24c256 at 0x50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4048.270884] bone_capemgr bone_capemgr: part_number 'BB-I2C1', version 'N/A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4048.278290] bone_capemgr bone_capemgr: slot #4: override</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4048.284097] bone_capemgr bone_capemgr: Using override eeprom data at slot 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4048.291286] bone_capemgr bone_capemgr: slot #4: 'Override Board Name,00A0,Override Manuf,BB-I2C1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.188638] bone_capemgr bone_capemgr: part_number 'duper-i2c', version 'N/A'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.209144] bone_capemgr bone_capemgr: slot #5: override</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.214676] bone_capemgr bone_capemgr: Using override eeprom data at slot 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.221766] bone_capemgr bone_capemgr: slot #5: 'Override Board Name,00A0,Override Manuf,duper-i2c'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.255983] i2c i2c-1: of_i2c: modalias failure on /ocp/i2c@4802a000/sdn@44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.270180] omap_i2c 4802a000.i2c: bus 1 rev0.11 at 100 kHz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4100.284051] bone_capemgr bone_capemgr: slot #5: dtbo 'duper-i2c-00A0.dtbo' loaded; overlay id #0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4241.191465] at24 1-0050: 32768 byte 24c256 EEPROM, writable, 1 bytes/write</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ 4241.210555] i2c i2c-1: new_device: Instantiated device 24c256 at 0x50</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">sudo cat /sys/bus/i2c/devices/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF3333"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">1-0050</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="TakaoGothic"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/eeprom | hexdump </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">[dmotooka@ *BBB* :~] </t>
+  </si>
 </sst>
 </file>
 
@@ -453,7 +631,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="TakaoPGothic"/>
@@ -497,6 +675,12 @@
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="TakaoPGothic"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <name val="TakaoGothic"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -556,7 +740,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,6 +758,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -660,9 +848,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>235800</xdr:colOff>
+      <xdr:colOff>235440</xdr:colOff>
       <xdr:row>53</xdr:row>
-      <xdr:rowOff>3960</xdr:rowOff>
+      <xdr:rowOff>3600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -671,13 +859,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="46425" t="28325" r="3630" b="0"/>
+        <a:srcRect l="46431" t="28329" r="3630" b="0"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16261200" y="1305000"/>
-          <a:ext cx="7977600" cy="7399440"/>
+          <a:ext cx="7977240" cy="7399080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -698,9 +886,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
-      <xdr:colOff>174240</xdr:colOff>
+      <xdr:colOff>173880</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -710,7 +898,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="24778080" y="4232880"/>
-          <a:ext cx="1456560" cy="2640600"/>
+          <a:ext cx="1456200" cy="2640240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -878,9 +1066,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>257400</xdr:colOff>
+      <xdr:colOff>257040</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>115200</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -889,13 +1077,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="25724" t="14121" r="37295" b="7013"/>
+        <a:srcRect l="25728" t="14124" r="37299" b="7013"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7990200" y="1485000"/>
-          <a:ext cx="5983200" cy="8143560"/>
+          <a:ext cx="5982840" cy="8143200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -916,9 +1104,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>339840</xdr:colOff>
+      <xdr:colOff>339480</xdr:colOff>
       <xdr:row>52</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -928,7 +1116,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="13970520" y="6805080"/>
-          <a:ext cx="1456920" cy="1807920"/>
+          <a:ext cx="1456560" cy="1807560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -996,9 +1184,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>116640</xdr:colOff>
+      <xdr:colOff>116280</xdr:colOff>
       <xdr:row>82</xdr:row>
-      <xdr:rowOff>16920</xdr:rowOff>
+      <xdr:rowOff>16560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1008,7 +1196,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4717800" y="11623680"/>
-          <a:ext cx="1571040" cy="1807920"/>
+          <a:ext cx="1570680" cy="1807560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1108,9 +1296,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>470160</xdr:colOff>
+      <xdr:colOff>469800</xdr:colOff>
       <xdr:row>98</xdr:row>
-      <xdr:rowOff>149040</xdr:rowOff>
+      <xdr:rowOff>148680</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1120,7 +1308,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5871600" y="14356800"/>
-          <a:ext cx="1456560" cy="1807920"/>
+          <a:ext cx="1456200" cy="1807560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1220,9 +1408,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>17280</xdr:colOff>
+      <xdr:colOff>16920</xdr:colOff>
       <xdr:row>156</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1232,7 +1420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6675840" y="23697000"/>
-          <a:ext cx="1571040" cy="1807920"/>
+          <a:ext cx="1570680" cy="1807560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1364,9 +1552,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>74160</xdr:colOff>
+      <xdr:colOff>73800</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>115200</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1375,13 +1563,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId8"/>
-        <a:srcRect l="33906" t="56777" r="29754" b="22621"/>
+        <a:srcRect l="33911" t="56784" r="29758" b="22625"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="676080"/>
-          <a:ext cx="6932160" cy="2125080"/>
+          <a:ext cx="6931800" cy="2124720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1402,9 +1590,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>219240</xdr:colOff>
+      <xdr:colOff>218880</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1413,13 +1601,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId9"/>
-        <a:srcRect l="35516" t="30303" r="30976" b="46425"/>
+        <a:srcRect l="35522" t="30306" r="30980" b="46432"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="3501720"/>
-          <a:ext cx="6391440" cy="2401920"/>
+          <a:ext cx="6391080" cy="2401560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1440,9 +1628,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>465120</xdr:colOff>
+      <xdr:colOff>464760</xdr:colOff>
       <xdr:row>51</xdr:row>
-      <xdr:rowOff>69120</xdr:rowOff>
+      <xdr:rowOff>68760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1451,13 +1639,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId10"/>
-        <a:srcRect l="34238" t="55423" r="30967" b="26352"/>
+        <a:srcRect l="34242" t="55430" r="30970" b="26355"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="6563880"/>
-          <a:ext cx="6637320" cy="1880640"/>
+          <a:ext cx="6636960" cy="1880280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1478,9 +1666,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>267840</xdr:colOff>
+      <xdr:colOff>267480</xdr:colOff>
       <xdr:row>172</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1490,7 +1678,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="686160" y="26583120"/>
-          <a:ext cx="6439680" cy="1491480"/>
+          <a:ext cx="6439320" cy="1491120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1595,9 +1783,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>592560</xdr:colOff>
+      <xdr:colOff>592200</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>148680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1606,13 +1794,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="30452" t="13893" r="21610" b="4239"/>
+        <a:srcRect l="30457" t="13893" r="21612" b="4239"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="335160" y="122040"/>
-          <a:ext cx="6658200" cy="7341840"/>
+          <a:ext cx="5743440" cy="7341480"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1626,16 +1814,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>763560</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>77760</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>48240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>624240</xdr:colOff>
+      <xdr:colOff>623880</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>18720</xdr:rowOff>
+      <xdr:rowOff>18360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1644,8 +1832,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7164360" y="4111920"/>
-          <a:ext cx="2260800" cy="946080"/>
+          <a:off x="6249960" y="4111920"/>
+          <a:ext cx="1917720" cy="945720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1777,9 +1965,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>673920</xdr:colOff>
+      <xdr:colOff>673560</xdr:colOff>
       <xdr:row>69</xdr:row>
-      <xdr:rowOff>133920</xdr:rowOff>
+      <xdr:rowOff>133560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1788,8 +1976,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="800640" y="10404360"/>
-          <a:ext cx="2273400" cy="946080"/>
+          <a:off x="686520" y="10404360"/>
+          <a:ext cx="2044440" cy="945720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1921,9 +2109,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>475200</xdr:colOff>
+      <xdr:colOff>474840</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1932,8 +2120,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8615880" y="10088640"/>
-          <a:ext cx="2260440" cy="946080"/>
+          <a:off x="7472880" y="10088640"/>
+          <a:ext cx="1917360" cy="945720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2038,9 +2226,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>534960</xdr:colOff>
+      <xdr:colOff>534600</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2049,13 +2237,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="22792" t="28049" r="10784" b="65535"/>
+        <a:srcRect l="22795" t="28052" r="10784" b="65542"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="488160"/>
-          <a:ext cx="8535960" cy="620640"/>
+          <a:ext cx="7392600" cy="620280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2076,9 +2264,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>445680</xdr:colOff>
+      <xdr:colOff>445320</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>84960</xdr:rowOff>
+      <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2087,13 +2275,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId2"/>
-        <a:srcRect l="23019" t="71442" r="11241" b="23127"/>
+        <a:srcRect l="23022" t="71449" r="11244" b="23131"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="1673280"/>
-          <a:ext cx="8446680" cy="524880"/>
+          <a:ext cx="7303320" cy="524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2114,9 +2302,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>158040</xdr:colOff>
+      <xdr:colOff>157680</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2125,13 +2313,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId3"/>
-        <a:srcRect l="23094" t="44476" r="7444" b="49602"/>
+        <a:srcRect l="23097" t="44480" r="7444" b="49606"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="39600" y="2782440"/>
-          <a:ext cx="8919360" cy="572760"/>
+          <a:ext cx="7661880" cy="572400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2157,9 +2345,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>593640</xdr:colOff>
+      <xdr:colOff>593280</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2168,13 +2356,13 @@
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:srcRect l="31218" t="27549" r="20499" b="9629"/>
+        <a:srcRect l="31223" t="27553" r="20502" b="9629"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="445680" y="152640"/>
-          <a:ext cx="6548760" cy="4924080"/>
+          <a:ext cx="5634000" cy="4923720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2582,6 +2770,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.58108108108108"/>
+  </cols>
   <sheetData>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
@@ -2659,6 +2850,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.58108108108108"/>
+  </cols>
   <sheetData>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
@@ -2694,11 +2888,14 @@
   </sheetPr>
   <dimension ref="A3:D181"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A150" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D162" activeCellId="0" sqref="D162"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A109" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E142" activeCellId="0" sqref="E142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.58108108108108"/>
+  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -2889,8 +3086,8 @@
       </c>
     </row>
     <row r="44" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="2" t="s">
+    <row r="46" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2966,16 +3163,16 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C57" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D57" s="4" t="s">
+      <c r="D57" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2995,7 +3192,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="5" t="s">
         <v>96</v>
       </c>
     </row>
@@ -3140,7 +3337,7 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="4" t="s">
+      <c r="A96" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3215,8 +3412,8 @@
       </c>
     </row>
     <row r="114" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="2" t="s">
+    <row r="115" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="4" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3226,7 +3423,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="4" t="s">
+      <c r="A118" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3264,7 +3461,7 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="4" t="s">
+      <c r="A123" s="5" t="s">
         <v>105</v>
       </c>
     </row>
@@ -3288,16 +3485,16 @@
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="4" t="s">
+      <c r="A126" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="B126" s="4" t="s">
+      <c r="B126" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3326,7 +3523,7 @@
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="4" t="s">
+      <c r="A131" s="5" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3561,7 +3758,7 @@
       </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="4" t="s">
+      <c r="A181" s="5" t="s">
         <v>115</v>
       </c>
     </row>
@@ -3581,6 +3778,411 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A2:D86"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1711711711712"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" s="3" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12ページ &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -3588,6 +4190,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.58108108108108"/>
+  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>